<commit_message>
Established County Investigation Strategy
</commit_message>
<xml_diff>
--- a/Data/ga_chronic_cond.xlsx
+++ b/Data/ga_chronic_cond.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamorgan/Documents/CourseWork/Spring20/Regression/Regression_Final_Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC926E8B-241A-A443-8600-6EED3CAE6189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE3913-5215-F248-98C4-B8BFDDE9690C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31880" yWindow="-2660" windowWidth="28040" windowHeight="17040" xr2:uid="{3D5FECE0-ECCA-994A-8A88-0CABE8C9896E}"/>
+    <workbookView xWindow="33960" yWindow="-3140" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{3D5FECE0-ECCA-994A-8A88-0CABE8C9896E}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="287">
   <si>
     <t>  SUBJECT AREA</t>
   </si>
@@ -844,13 +844,64 @@
   </si>
   <si>
     <t>85.7, 90.1</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>DEM_CAT</t>
+  </si>
+  <si>
+    <t>DEM_GROUP</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>BLACK</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>HISP</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>18-24</t>
+  </si>
+  <si>
+    <t>INCOME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -884,6 +935,12 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -905,12 +962,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1227,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B047C3DF-B9D8-8147-A0C5-03FF75E3939F}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93:C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3904,12 +3967,1168 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90FFCF1-F613-D544-A993-B60CF0FCF4BE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F55" sqref="A1:F55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="2">
+        <v>11.8</v>
+      </c>
+      <c r="E2">
+        <v>10.4</v>
+      </c>
+      <c r="F2">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="E3">
+        <v>11.1</v>
+      </c>
+      <c r="F3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="E4">
+        <v>11.3</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="E5">
+        <v>11.4</v>
+      </c>
+      <c r="F5">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E6">
+        <v>3.3</v>
+      </c>
+      <c r="F6">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>2.6</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4.2</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F10">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2">
+        <v>14.4</v>
+      </c>
+      <c r="E11">
+        <v>11.8</v>
+      </c>
+      <c r="F11">
+        <v>17.3</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="E12">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F12">
+        <v>23.4</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="E13">
+        <v>24.7</v>
+      </c>
+      <c r="F13">
+        <v>29.8</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E14">
+        <v>15.1</v>
+      </c>
+      <c r="F14">
+        <v>23.4</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14.2</v>
+      </c>
+      <c r="E15">
+        <v>11.7</v>
+      </c>
+      <c r="F15">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="E16">
+        <v>11.3</v>
+      </c>
+      <c r="F16">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2">
+        <v>15.9</v>
+      </c>
+      <c r="E17">
+        <v>12.6</v>
+      </c>
+      <c r="F17">
+        <v>19.8</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="E18">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F18">
+        <v>14.1</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="E19">
+        <v>5.5</v>
+      </c>
+      <c r="F19">
+        <v>8.6</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>276</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F20">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="E21" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F21">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>7.8</v>
+      </c>
+      <c r="F22">
+        <v>10.5</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s">
+        <v>279</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.4</v>
+      </c>
+      <c r="E23">
+        <v>7.6</v>
+      </c>
+      <c r="F23">
+        <v>11.7</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" t="s">
+        <v>279</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="E24">
+        <v>2.6</v>
+      </c>
+      <c r="F24">
+        <v>8.9</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>9.5</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9.4</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>14.3</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>284</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="E27">
+        <v>5.7</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="E28">
+        <v>5.9</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>284</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="E29">
+        <v>7.4</v>
+      </c>
+      <c r="F29">
+        <v>12.2</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="E30">
+        <v>7.5</v>
+      </c>
+      <c r="F30">
+        <v>11.9</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="E31">
+        <v>5.8</v>
+      </c>
+      <c r="F31">
+        <v>8.6</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>286</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E32">
+        <v>11.3</v>
+      </c>
+      <c r="F32">
+        <v>20.8</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" t="s">
+        <v>286</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E33">
+        <v>6.8</v>
+      </c>
+      <c r="F33">
+        <v>12.3</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" t="s">
+        <v>286</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="2">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
+        <v>286</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="E35">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F35">
+        <v>10.4</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E36">
+        <v>3.6</v>
+      </c>
+      <c r="F36">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="E37">
+        <v>5.4</v>
+      </c>
+      <c r="F37">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D38" s="4">
+        <v>39.9</v>
+      </c>
+      <c r="E38">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="F38">
+        <v>42.6</v>
+      </c>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39" t="s">
+        <v>276</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D39" s="4">
+        <v>28.8</v>
+      </c>
+      <c r="E39">
+        <v>26.6</v>
+      </c>
+      <c r="F39">
+        <v>31.1</v>
+      </c>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" t="s">
+        <v>279</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D40" s="4">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E40">
+        <v>32.5</v>
+      </c>
+      <c r="F40">
+        <v>36.9</v>
+      </c>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D41" s="4">
+        <v>32.6</v>
+      </c>
+      <c r="E41">
+        <v>29.3</v>
+      </c>
+      <c r="F41">
+        <v>36</v>
+      </c>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" t="s">
+        <v>279</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D42" s="4">
+        <v>35.6</v>
+      </c>
+      <c r="E42">
+        <v>28</v>
+      </c>
+      <c r="F42">
+        <v>44</v>
+      </c>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43" t="s">
+        <v>279</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D43" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E43">
+        <v>30.8</v>
+      </c>
+      <c r="F43">
+        <v>46.2</v>
+      </c>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" t="s">
+        <v>284</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D44" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="E44">
+        <v>17</v>
+      </c>
+      <c r="F44">
+        <v>27.3</v>
+      </c>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="4">
+        <v>34.1</v>
+      </c>
+      <c r="E45">
+        <v>29.5</v>
+      </c>
+      <c r="F45">
+        <v>39.1</v>
+      </c>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" t="s">
+        <v>284</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="4">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E46">
+        <v>30.1</v>
+      </c>
+      <c r="F46">
+        <v>39.6</v>
+      </c>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="4">
+        <v>39.4</v>
+      </c>
+      <c r="E47">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F47">
+        <v>43.6</v>
+      </c>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" t="s">
+        <v>284</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="4">
+        <v>37.1</v>
+      </c>
+      <c r="E48">
+        <v>33.4</v>
+      </c>
+      <c r="F48">
+        <v>41</v>
+      </c>
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>211</v>
+      </c>
+      <c r="B49" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="4">
+        <v>36.4</v>
+      </c>
+      <c r="E49">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="F49">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" t="s">
+        <v>286</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="4">
+        <v>27.9</v>
+      </c>
+      <c r="E50">
+        <v>22.8</v>
+      </c>
+      <c r="F50">
+        <v>33.6</v>
+      </c>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" t="s">
+        <v>286</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="4">
+        <v>31.1</v>
+      </c>
+      <c r="E51">
+        <v>27</v>
+      </c>
+      <c r="F51">
+        <v>35.4</v>
+      </c>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" t="s">
+        <v>286</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="4">
+        <v>38.6</v>
+      </c>
+      <c r="E52">
+        <v>32.5</v>
+      </c>
+      <c r="F52">
+        <v>44.9</v>
+      </c>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B53" t="s">
+        <v>286</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="4">
+        <v>30.4</v>
+      </c>
+      <c r="E53">
+        <v>25.9</v>
+      </c>
+      <c r="F53">
+        <v>35.4</v>
+      </c>
+      <c r="G53" s="4"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>211</v>
+      </c>
+      <c r="B54" t="s">
+        <v>286</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="4">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E54">
+        <v>29.5</v>
+      </c>
+      <c r="F54">
+        <v>39.5</v>
+      </c>
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>211</v>
+      </c>
+      <c r="B55" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="4">
+        <v>39.1</v>
+      </c>
+      <c r="E55">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="F55">
+        <v>42.6</v>
+      </c>
+      <c r="G55" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>